<commit_message>
added weighted average line
</commit_message>
<xml_diff>
--- a/ddd_feb_2.xlsx
+++ b/ddd_feb_2.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LinBin/Documents/repos/ID_submission/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FE0643-82B3-204B-A271-ADF4A69A613E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDD per Location" sheetId="1" r:id="rId1"/>
     <sheet name="DDD per Department" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -29,9 +35,6 @@
     <t>LOC_NAME</t>
   </si>
   <si>
-    <t>DOT_VALUE</t>
-  </si>
-  <si>
     <t>Patient Days</t>
   </si>
   <si>
@@ -111,16 +114,19 @@
   </si>
   <si>
     <t>MM 3B1 EAT DISORDERS</t>
+  </si>
+  <si>
+    <t>DDD_VALUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +190,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -230,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,9 +276,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,6 +328,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -471,14 +521,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,27 +544,27 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44197</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -524,18 +576,18 @@
         <v>5.390835</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44228</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -547,18 +599,18 @@
         <v>20.637898</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44256</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -567,21 +619,21 @@
         <v>772</v>
       </c>
       <c r="G4">
-        <v>7.77202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>7.7720200000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44287</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -590,21 +642,21 @@
         <v>985</v>
       </c>
       <c r="G5">
-        <v>4.060913</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>4.0609130000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44317</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6">
         <v>9</v>
@@ -613,21 +665,21 @@
         <v>1692</v>
       </c>
       <c r="G6">
-        <v>5.319148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>5.3191480000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44348</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -639,18 +691,18 @@
         <v>27.777777</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44348</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>7</v>
@@ -659,21 +711,21 @@
         <v>1539</v>
       </c>
       <c r="G8">
-        <v>4.548408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>4.5484080000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44378</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -682,21 +734,21 @@
         <v>226</v>
       </c>
       <c r="G9">
-        <v>4.424778</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>4.4247779999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44378</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -705,21 +757,21 @@
         <v>713</v>
       </c>
       <c r="G10">
-        <v>1.402524</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>1.4025240000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44409</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -728,21 +780,21 @@
         <v>958</v>
       </c>
       <c r="G11">
-        <v>3.131524</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>3.1315240000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44409</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -754,18 +806,18 @@
         <v>13.333333</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44440</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -774,21 +826,21 @@
         <v>293</v>
       </c>
       <c r="G13">
-        <v>6.825938</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>6.8259379999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44440</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -797,21 +849,21 @@
         <v>76</v>
       </c>
       <c r="G14">
-        <v>26.315789</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>26.315788999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44440</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -820,21 +872,21 @@
         <v>420</v>
       </c>
       <c r="G15">
-        <v>16.666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>16.666665999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44470</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -843,21 +895,21 @@
         <v>186</v>
       </c>
       <c r="G16">
-        <v>10.752688</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>10.752687999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44470</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -866,21 +918,21 @@
         <v>279</v>
       </c>
       <c r="G17">
-        <v>3.584229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>3.5842290000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44470</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -889,21 +941,21 @@
         <v>467</v>
       </c>
       <c r="G18">
-        <v>4.282655</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>4.2826550000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44501</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -912,21 +964,21 @@
         <v>60</v>
       </c>
       <c r="G19">
-        <v>16.666666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>16.666665999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44531</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -935,7 +987,7 @@
         <v>737</v>
       </c>
       <c r="G20">
-        <v>2.713704</v>
+        <v>2.7137039999999999</v>
       </c>
     </row>
   </sheetData>
@@ -944,14 +996,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,33 +1019,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44197</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1000,24 +1054,24 @@
         <v>526</v>
       </c>
       <c r="H2">
-        <v>1.90114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>1.9011400000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44197</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1029,21 +1083,21 @@
         <v>13.888888</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44228</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1052,24 +1106,24 @@
         <v>201</v>
       </c>
       <c r="H4">
-        <v>4.975124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>4.9751240000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44228</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1081,21 +1135,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44228</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>7</v>
@@ -1107,21 +1161,21 @@
         <v>25.735294</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44256</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -1130,24 +1184,24 @@
         <v>463</v>
       </c>
       <c r="H7">
-        <v>4.319654</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>4.3196539999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44256</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -1156,24 +1210,24 @@
         <v>309</v>
       </c>
       <c r="H8">
-        <v>12.944983</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>12.944983000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44287</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1185,21 +1239,21 @@
         <v>1.477104</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44287</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -1211,21 +1265,21 @@
         <v>9.740259</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44317</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -1234,24 +1288,24 @@
         <v>1321</v>
       </c>
       <c r="H11">
-        <v>3.785011</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>3.7850109999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44317</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -1260,24 +1314,24 @@
         <v>371</v>
       </c>
       <c r="H12">
-        <v>10.781671</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>10.781670999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>44348</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -1286,24 +1340,24 @@
         <v>1215</v>
       </c>
       <c r="H13">
-        <v>2.469135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>2.4691350000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>44348</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1312,24 +1366,24 @@
         <v>324</v>
       </c>
       <c r="H14">
-        <v>12.345679</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>12.345679000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>44348</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1341,21 +1395,21 @@
         <v>27.777777</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>44378</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1364,24 +1418,24 @@
         <v>713</v>
       </c>
       <c r="H16">
-        <v>1.402524</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>1.4025240000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>44378</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1390,24 +1444,24 @@
         <v>226</v>
       </c>
       <c r="H17">
-        <v>4.424778</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>4.4247779999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>44409</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1419,21 +1473,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>44409</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1442,24 +1496,24 @@
         <v>110</v>
       </c>
       <c r="H19">
-        <v>9.090909</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>9.0909089999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>44409</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1468,24 +1522,24 @@
         <v>348</v>
       </c>
       <c r="H20">
-        <v>2.873563</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>2.8735629999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>44409</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -1494,24 +1548,24 @@
         <v>553</v>
       </c>
       <c r="H21">
-        <v>1.808318</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>1.8083180000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>44409</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1520,24 +1574,24 @@
         <v>57</v>
       </c>
       <c r="H22">
-        <v>17.543859</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>17.543859000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>44440</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1546,24 +1600,24 @@
         <v>188</v>
       </c>
       <c r="H23">
-        <v>5.319148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>5.3191480000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>44440</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1575,21 +1629,21 @@
         <v>9.523809</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>44440</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25">
         <v>2</v>
@@ -1598,24 +1652,24 @@
         <v>76</v>
       </c>
       <c r="H25">
-        <v>26.315789</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>26.315788999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>44440</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F26">
         <v>4</v>
@@ -1624,24 +1678,24 @@
         <v>38</v>
       </c>
       <c r="H26">
-        <v>105.263157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>105.26315700000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>44440</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -1650,24 +1704,24 @@
         <v>382</v>
       </c>
       <c r="H27">
-        <v>7.853403</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>7.8534030000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>44470</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28">
         <v>2</v>
@@ -1676,24 +1730,24 @@
         <v>186</v>
       </c>
       <c r="H28">
-        <v>10.752688</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>10.752687999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>44470</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1702,24 +1756,24 @@
         <v>279</v>
       </c>
       <c r="H29">
-        <v>3.584229</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>3.5842290000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>44470</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1728,24 +1782,24 @@
         <v>62</v>
       </c>
       <c r="H30">
-        <v>16.129032</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>16.129031999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>44470</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1754,24 +1808,24 @@
         <v>405</v>
       </c>
       <c r="H31">
-        <v>2.469135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>2.4691350000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>44501</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1780,24 +1834,24 @@
         <v>60</v>
       </c>
       <c r="H32">
-        <v>16.666666</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>16.666665999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>44531</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -1806,7 +1860,7 @@
         <v>737</v>
       </c>
       <c r="H33">
-        <v>2.713704</v>
+        <v>2.7137039999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>